<commit_message>
update document de planif
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/DocumentDePlanification.xlsx
+++ b/DOCUMENTATION/DocumentDePlanification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxxr\Documents\GitHub\C61-MaximeRabbat-AbigailFournier\DOCUMENTATION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fourn\OneDrive\Documents\GitHub\C61-MaximeRabbat-AbigailFournier\DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED09608D-F5C0-4962-9CC6-5403FC140C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D51799-1E09-47B7-AB95-8F3A21895808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planification" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="99">
   <si>
     <t>Planification globale</t>
   </si>
@@ -298,9 +298,6 @@
     <t>Compréhension de base de son fonctionnement</t>
   </si>
   <si>
-    <t>c'étit compliqué à placer</t>
-  </si>
-  <si>
     <t>non commencé</t>
   </si>
   <si>
@@ -317,6 +314,18 @@
   </si>
   <si>
     <t>Manqué de temp et moins prioritaire</t>
+  </si>
+  <si>
+    <t>c'était compliqué à placer</t>
+  </si>
+  <si>
+    <t>Beaucoup de découverte de ce qui est possible ou pas</t>
+  </si>
+  <si>
+    <t>Beaucoup d'erreurs et d'échec d'essai d'effets</t>
+  </si>
+  <si>
+    <t>Petit survol</t>
   </si>
 </sst>
 </file>
@@ -520,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -559,6 +568,7 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -4214,7 +4224,7 @@
   <dimension ref="B1:L1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4347,7 +4357,7 @@
         <v>100</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J6" s="34">
         <v>0</v>
@@ -4409,7 +4419,7 @@
         <v>50</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J8">
         <v>4</v>
@@ -4418,7 +4428,7 @@
         <v>90</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -4454,7 +4464,7 @@
     </row>
     <row r="10" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>66</v>
@@ -4566,7 +4576,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J13" s="34">
         <v>2</v>
@@ -4575,7 +4585,7 @@
         <v>100</v>
       </c>
       <c r="L13" s="27" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -4621,6 +4631,9 @@
       <c r="D15" s="33">
         <v>0</v>
       </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
       <c r="F15" s="32"/>
       <c r="G15" s="33">
         <v>0</v>
@@ -4636,20 +4649,30 @@
         <v>66</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16" s="17"/>
+        <v>25</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>98</v>
+      </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I16" s="17"/>
-      <c r="L16" s="17"/>
+      <c r="J16" s="35">
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>75</v>
+      </c>
+      <c r="L16" s="17" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="17" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
@@ -4672,7 +4695,15 @@
         <v>0</v>
       </c>
       <c r="I17" s="17"/>
-      <c r="L17" s="17"/>
+      <c r="J17" s="35">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>100</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="18" spans="2:12" s="30" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
@@ -4731,7 +4762,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -4762,7 +4793,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -4793,7 +4824,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -4824,7 +4855,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -4855,7 +4886,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
document de planif update
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/DocumentDePlanification.xlsx
+++ b/DOCUMENTATION/DocumentDePlanification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxxr\Documents\GitHub\C61-MaximeRabbat-AbigailFournier\DOCUMENTATION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fourn\OneDrive\Documents\GitHub\C61-MaximeRabbat-AbigailFournier\DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E171D651-8161-4AF1-BB79-1235FC1E7D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0305CEE3-B362-4903-9F2D-41BBAB8EAC96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planification" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="146">
   <si>
     <t>Planification globale</t>
   </si>
@@ -391,22 +391,82 @@
     <t>Level Node</t>
   </si>
   <si>
-    <t xml:space="preserve">Finir ennemies </t>
-  </si>
-  <si>
-    <t>Création de Interactive Object</t>
-  </si>
-  <si>
     <t>Création de Tool</t>
   </si>
   <si>
-    <t xml:space="preserve">Création de Obstacle </t>
-  </si>
-  <si>
     <t>Level Start</t>
   </si>
   <si>
     <t>niveaux ne sont pas tous existant encore</t>
+  </si>
+  <si>
+    <t>Level Switch Animation (fadeIn fadeOut)</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Création de Obstacle  (light spheres, boxes)</t>
+  </si>
+  <si>
+    <t>Dialogues</t>
+  </si>
+  <si>
+    <t>Inventory HUD</t>
+  </si>
+  <si>
+    <t>Eyes of Ra (HUD + battery + toggle on/off with R )</t>
+  </si>
+  <si>
+    <t>Glider</t>
+  </si>
+  <si>
+    <t>Light grenades</t>
+  </si>
+  <si>
+    <t>Chromas touch (infinite eyes of ra power)</t>
+  </si>
+  <si>
+    <t>Final puzzle (colored levers and buttons / pipes )</t>
+  </si>
+  <si>
+    <t>Final sun lighting up animation</t>
+  </si>
+  <si>
+    <t>Création de Interactive Object (levers, buttons, pressure plates, door)</t>
+  </si>
+  <si>
+    <t>Lit up zone indicator (for grenades or eyes of ra)</t>
+  </si>
+  <si>
+    <t>Finir ennemies (Animations and flying ennemy coroutine)</t>
+  </si>
+  <si>
+    <t>Collectibles (keys + battery / firefly pickup)</t>
+  </si>
+  <si>
+    <t>Bridges appear when level completed</t>
+  </si>
+  <si>
+    <t>3d background house that can be entered for final level / puzzle</t>
+  </si>
+  <si>
+    <t>HUD for level completion</t>
+  </si>
+  <si>
+    <t>Controls to restart levels or go back to level select / main menu</t>
+  </si>
+  <si>
+    <t>incorporate sound / music</t>
+  </si>
+  <si>
+    <t>Rocket boots / Light jump (light trail)</t>
+  </si>
+  <si>
+    <t>Max / Abi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max   </t>
   </si>
 </sst>
 </file>
@@ -414,7 +474,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;$&quot;_);[Red]\(#,##0.00\ &quot;$&quot;\)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;$&quot;_);[Red]\(#,##0.00\ &quot;$&quot;\)"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -495,7 +555,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -613,6 +673,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -790,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -839,7 +923,7 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="4" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -862,10 +946,20 @@
     <xf numFmtId="0" fontId="11" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1088,11 +1182,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1029"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.109375" customWidth="1"/>
     <col min="2" max="2" width="47.44140625" customWidth="1"/>
@@ -3037,7 +3131,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.88671875" customWidth="1"/>
     <col min="2" max="2" width="51.6640625" customWidth="1"/>
@@ -4528,7 +4622,7 @@
       <selection activeCell="B20" sqref="B20:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.33203125" customWidth="1"/>
     <col min="2" max="2" width="42.21875" customWidth="1"/>
@@ -6320,11 +6414,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="95" workbookViewId="0">
+    <sheetView zoomScale="95" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.88671875" customWidth="1"/>
     <col min="2" max="2" width="50.77734375" customWidth="1"/>
@@ -9445,13 +9539,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B1:O1002"/>
+  <dimension ref="B1:O1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.6640625" customWidth="1"/>
     <col min="2" max="2" width="68.88671875" customWidth="1"/>
@@ -9545,7 +9639,9 @@
       </c>
     </row>
     <row r="5" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B5" s="23"/>
+      <c r="B5" s="70" t="s">
+        <v>123</v>
+      </c>
       <c r="C5" s="17"/>
       <c r="F5" s="17"/>
       <c r="I5" s="17"/>
@@ -9553,39 +9649,57 @@
       <c r="O5" s="17"/>
     </row>
     <row r="6" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B6" s="23"/>
-      <c r="C6" s="17"/>
+      <c r="B6" s="67" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="65" t="s">
+        <v>144</v>
+      </c>
       <c r="F6" s="17"/>
       <c r="I6" s="17"/>
       <c r="L6" s="17"/>
       <c r="O6" s="17"/>
     </row>
     <row r="7" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
-      <c r="C7" s="17"/>
+      <c r="B7" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>144</v>
+      </c>
       <c r="F7" s="17"/>
       <c r="I7" s="17"/>
       <c r="L7" s="17"/>
       <c r="O7" s="17"/>
     </row>
     <row r="8" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-      <c r="C8" s="17"/>
+      <c r="B8" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>66</v>
+      </c>
       <c r="F8" s="17"/>
       <c r="I8" s="17"/>
       <c r="L8" s="17"/>
       <c r="O8" s="17"/>
     </row>
     <row r="9" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B9" s="23"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>66</v>
+      </c>
       <c r="F9" s="17"/>
       <c r="I9" s="17"/>
       <c r="L9" s="17"/>
       <c r="O9" s="17"/>
     </row>
     <row r="10" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
+      <c r="B10" s="70" t="s">
+        <v>131</v>
+      </c>
       <c r="C10" s="17"/>
       <c r="F10" s="17"/>
       <c r="I10" s="17"/>
@@ -9593,7 +9707,9 @@
       <c r="O10" s="17"/>
     </row>
     <row r="11" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="23"/>
+      <c r="B11" s="70" t="s">
+        <v>132</v>
+      </c>
       <c r="C11" s="17"/>
       <c r="F11" s="17"/>
       <c r="I11" s="17"/>
@@ -9601,7 +9717,9 @@
       <c r="O11" s="17"/>
     </row>
     <row r="12" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B12" s="23"/>
+      <c r="B12" s="74" t="s">
+        <v>133</v>
+      </c>
       <c r="C12" s="17"/>
       <c r="F12" s="17"/>
       <c r="I12" s="17"/>
@@ -9609,54 +9727,64 @@
       <c r="O12" s="17"/>
     </row>
     <row r="13" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B13" s="23"/>
-      <c r="C13" s="17"/>
+      <c r="B13" s="75" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="65" t="s">
+        <v>145</v>
+      </c>
       <c r="F13" s="17"/>
       <c r="I13" s="17"/>
       <c r="L13" s="17"/>
       <c r="O13" s="17"/>
     </row>
     <row r="14" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B14" s="23"/>
-      <c r="C14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="O14" s="17"/>
-    </row>
-    <row r="15" spans="2:15" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B15" s="62" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="L15" s="63"/>
-      <c r="O15" s="63"/>
+      <c r="B14" s="76" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="O14" s="27"/>
+    </row>
+    <row r="15" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B15" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="O15" s="27"/>
     </row>
     <row r="16" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B16" s="65" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="O16" s="17"/>
+      <c r="B16" s="75" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="O16" s="27"/>
     </row>
     <row r="17" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B17" s="65" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="O17" s="17"/>
+      <c r="B17" s="75" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="O17" s="27"/>
     </row>
     <row r="18" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B18" s="65" t="s">
-        <v>117</v>
+      <c r="B18" s="70" t="s">
+        <v>142</v>
       </c>
       <c r="C18" s="17"/>
       <c r="F18" s="17"/>
@@ -9664,18 +9792,20 @@
       <c r="L18" s="17"/>
       <c r="O18" s="17"/>
     </row>
-    <row r="19" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B19" s="65" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="O19" s="17"/>
+    <row r="19" spans="2:15" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B19" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="O19" s="63"/>
     </row>
     <row r="20" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B20" s="23"/>
+      <c r="B20" s="71" t="s">
+        <v>115</v>
+      </c>
       <c r="C20" s="17"/>
       <c r="F20" s="17"/>
       <c r="I20" s="17"/>
@@ -9683,53 +9813,36 @@
       <c r="O20" s="17"/>
     </row>
     <row r="21" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B21" s="67" t="s">
-        <v>124</v>
-      </c>
-      <c r="C21" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21">
-        <v>50</v>
-      </c>
-      <c r="F21" s="68" t="s">
-        <v>125</v>
-      </c>
-      <c r="I21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="O21" s="27"/>
+      <c r="B21" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="O21" s="17"/>
     </row>
     <row r="22" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B22" s="67" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22">
-        <v>100</v>
-      </c>
-      <c r="F22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="O22" s="27"/>
-    </row>
-    <row r="23" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="65" t="s">
-        <v>119</v>
-      </c>
-      <c r="C23" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23">
-        <v>100</v>
-      </c>
+      <c r="B22" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="O22" s="17"/>
+    </row>
+    <row r="23" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B23" s="71" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="17"/>
       <c r="F23" s="17"/>
       <c r="I23" s="17"/>
       <c r="L23" s="17"/>
       <c r="O23" s="17"/>
     </row>
-    <row r="24" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B24" s="23"/>
       <c r="C24" s="17"/>
       <c r="F24" s="17"/>
@@ -9737,40 +9850,55 @@
       <c r="L24" s="17"/>
       <c r="O24" s="17"/>
     </row>
-    <row r="25" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="65" t="s">
+    <row r="25" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B25" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="O25" s="17"/>
-    </row>
-    <row r="26" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="65" t="s">
+      <c r="C25" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25">
+        <v>50</v>
+      </c>
+      <c r="F25" s="66" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="O26" s="17"/>
+      <c r="I25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="O25" s="27"/>
+    </row>
+    <row r="26" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B26" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+      <c r="F26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="O26" s="27"/>
     </row>
     <row r="27" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="65" t="s">
-        <v>123</v>
-      </c>
-      <c r="C27" s="17"/>
+      <c r="B27" s="78" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27">
+        <v>100</v>
+      </c>
       <c r="F27" s="17"/>
       <c r="I27" s="17"/>
       <c r="L27" s="17"/>
       <c r="O27" s="17"/>
     </row>
     <row r="28" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="65" t="s">
-        <v>120</v>
-      </c>
+      <c r="B28" s="23"/>
       <c r="C28" s="17"/>
       <c r="F28" s="17"/>
       <c r="I28" s="17"/>
@@ -9778,15 +9906,21 @@
       <c r="O28" s="17"/>
     </row>
     <row r="29" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="23"/>
-      <c r="C29" s="17"/>
+      <c r="B29" s="69" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="65" t="s">
+        <v>144</v>
+      </c>
       <c r="F29" s="17"/>
       <c r="I29" s="17"/>
       <c r="L29" s="17"/>
       <c r="O29" s="17"/>
     </row>
     <row r="30" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="23"/>
+      <c r="B30" s="71" t="s">
+        <v>120</v>
+      </c>
       <c r="C30" s="17"/>
       <c r="F30" s="17"/>
       <c r="I30" s="17"/>
@@ -9794,48 +9928,68 @@
       <c r="O30" s="17"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="23"/>
-      <c r="C31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="O31" s="17"/>
+      <c r="B31" s="68" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="O31" s="27"/>
     </row>
     <row r="32" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="23"/>
-      <c r="C32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="O32" s="17"/>
+      <c r="B32" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="L32" s="27"/>
+      <c r="O32" s="27"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="23"/>
-      <c r="C33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="L33" s="17"/>
-      <c r="O33" s="17"/>
+      <c r="B33" s="72" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="L33" s="27"/>
+      <c r="O33" s="27"/>
     </row>
     <row r="34" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="23"/>
-      <c r="C34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="O34" s="17"/>
+      <c r="B34" s="68" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="O34" s="27"/>
     </row>
     <row r="35" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="23"/>
-      <c r="C35" s="17"/>
+      <c r="B35" s="69" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="65" t="s">
+        <v>56</v>
+      </c>
       <c r="F35" s="17"/>
       <c r="I35" s="17"/>
       <c r="L35" s="17"/>
       <c r="O35" s="17"/>
     </row>
     <row r="36" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="23"/>
-      <c r="C36" s="17"/>
+      <c r="B36" s="69" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="65" t="s">
+        <v>56</v>
+      </c>
       <c r="F36" s="17"/>
       <c r="I36" s="17"/>
       <c r="L36" s="17"/>
@@ -9897,27 +10051,83 @@
       <c r="L43" s="17"/>
       <c r="O43" s="17"/>
     </row>
-    <row r="44" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="23"/>
+      <c r="C44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="O44" s="17"/>
+    </row>
+    <row r="45" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="23"/>
+      <c r="C45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="O45" s="17"/>
+    </row>
+    <row r="46" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="23"/>
+      <c r="C46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="O46" s="17"/>
+    </row>
+    <row r="47" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="23"/>
+      <c r="C47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="O47" s="17"/>
+    </row>
+    <row r="48" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="23"/>
+      <c r="C48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="O48" s="17"/>
+    </row>
+    <row r="49" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="23"/>
+      <c r="C49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="O49" s="17"/>
+    </row>
+    <row r="50" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="23"/>
+      <c r="C50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="O50" s="17"/>
+    </row>
+    <row r="51" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="23"/>
+      <c r="C51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="O51" s="17"/>
+    </row>
+    <row r="52" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10856,6 +11066,14 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Planification Global Sprint 4
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/DocumentDePlanification.xlsx
+++ b/DOCUMENTATION/DocumentDePlanification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxxr\Documents\GitHub\C61-MaximeRabbat-AbigailFournier\DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE897EA-10C4-417B-9C0C-986A1C6A75A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BF4896-C7C6-4C19-82E5-85761023A375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planification" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="173">
   <si>
     <t>Planification globale</t>
   </si>
@@ -502,9 +502,6 @@
     <t>do we really nead em ?</t>
   </si>
   <si>
-    <t>easy to abes</t>
-  </si>
-  <si>
     <t>menu loads current level progress(untested)</t>
   </si>
   <si>
@@ -518,6 +515,39 @@
   </si>
   <si>
     <t xml:space="preserve">Background Parallax </t>
+  </si>
+  <si>
+    <t>battery fixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">was not added </t>
+  </si>
+  <si>
+    <t>works</t>
+  </si>
+  <si>
+    <t>Fully Functional</t>
+  </si>
+  <si>
+    <t>we did not do them</t>
+  </si>
+  <si>
+    <t>easily implemented</t>
+  </si>
+  <si>
+    <t>added light ball</t>
+  </si>
+  <si>
+    <t>ran out of time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remembers most things </t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>progressive music</t>
   </si>
 </sst>
 </file>
@@ -925,7 +955,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1011,6 +1041,7 @@
     <xf numFmtId="0" fontId="4" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="24" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9592,8 +9623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:O1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="F20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9694,16 +9725,36 @@
         <v>123</v>
       </c>
       <c r="C5" s="17"/>
+      <c r="D5">
+        <v>0</v>
+      </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" s="17"/>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
       <c r="I5" s="17"/>
+      <c r="J5" s="79">
+        <v>0</v>
+      </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" s="17"/>
-      <c r="O5" s="17"/>
+      <c r="M5" s="79">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="6" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="67" t="s">
@@ -9712,18 +9763,38 @@
       <c r="C6" s="65" t="s">
         <v>144</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" s="17"/>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
       <c r="I6" s="17"/>
+      <c r="J6" s="79">
+        <v>1</v>
+      </c>
       <c r="K6">
         <v>20</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="O6" s="17"/>
+        <v>157</v>
+      </c>
+      <c r="M6" s="79">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>80</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="7" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B7" s="67" t="s">
@@ -9732,18 +9803,38 @@
       <c r="C7" s="65" t="s">
         <v>144</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" s="17"/>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
       <c r="I7" s="17"/>
+      <c r="J7" s="79">
+        <v>2</v>
+      </c>
       <c r="K7">
         <v>70</v>
       </c>
       <c r="L7" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="O7" s="17"/>
+      <c r="M7" s="79">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>100</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="8" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B8" s="67" t="s">
@@ -9752,16 +9843,34 @@
       <c r="C8" s="65" t="s">
         <v>66</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" s="17"/>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
       <c r="I8" s="17"/>
+      <c r="J8" s="79">
+        <v>2</v>
+      </c>
       <c r="K8">
         <v>80</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
+      </c>
+      <c r="M8" s="79">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>100</v>
       </c>
       <c r="O8" s="17"/>
     </row>
@@ -9772,15 +9881,33 @@
       <c r="C9" s="65" t="s">
         <v>66</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9" s="17"/>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
       <c r="I9" s="17"/>
+      <c r="J9" s="79">
+        <v>3</v>
+      </c>
       <c r="K9">
         <v>100</v>
       </c>
       <c r="L9" s="17"/>
+      <c r="M9" s="79">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>100</v>
+      </c>
       <c r="O9" s="17"/>
     </row>
     <row r="10" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -9788,52 +9915,110 @@
         <v>131</v>
       </c>
       <c r="C10" s="17"/>
+      <c r="D10">
+        <v>0</v>
+      </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" s="17"/>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
       <c r="I10" s="17"/>
+      <c r="J10" s="79">
+        <v>0</v>
+      </c>
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="O10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="79">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>100</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="11" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B11" s="70" t="s">
         <v>132</v>
       </c>
       <c r="C11" s="17"/>
+      <c r="D11">
+        <v>0</v>
+      </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" s="17"/>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
       <c r="I11" s="17"/>
+      <c r="J11" s="79">
+        <v>2</v>
+      </c>
       <c r="K11">
         <v>50</v>
       </c>
       <c r="L11" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="O11" s="17"/>
+      <c r="M11" s="79">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>100</v>
+      </c>
+      <c r="O11" s="17" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="12" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B12" s="74" t="s">
         <v>133</v>
       </c>
       <c r="C12" s="17"/>
+      <c r="D12">
+        <v>0</v>
+      </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" s="17"/>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
       <c r="I12" s="17"/>
+      <c r="J12" s="79">
+        <v>0</v>
+      </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12" s="17"/>
-      <c r="O12" s="17"/>
+      <c r="M12" s="79">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="17" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="13" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B13" s="75" t="s">
@@ -9842,15 +10027,33 @@
       <c r="C13" s="65" t="s">
         <v>145</v>
       </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13" s="17"/>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
       <c r="I13" s="17"/>
+      <c r="J13" s="79">
+        <v>1</v>
+      </c>
       <c r="K13">
         <v>100</v>
       </c>
       <c r="L13" s="17"/>
+      <c r="M13" s="79">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>100</v>
+      </c>
       <c r="O13" s="17"/>
     </row>
     <row r="14" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -9858,32 +10061,72 @@
         <v>138</v>
       </c>
       <c r="C14" s="27"/>
+      <c r="D14">
+        <v>0</v>
+      </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" s="27"/>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
       <c r="I14" s="27"/>
+      <c r="J14" s="79">
+        <v>0</v>
+      </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14" s="27"/>
-      <c r="O14" s="27"/>
+      <c r="M14" s="79">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" s="27" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="15" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B15" s="73" t="s">
         <v>139</v>
       </c>
       <c r="C15" s="27"/>
+      <c r="D15">
+        <v>0</v>
+      </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15" s="27"/>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
       <c r="I15" s="27"/>
+      <c r="J15" s="79">
+        <v>0</v>
+      </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15" s="27"/>
-      <c r="O15" s="27"/>
+      <c r="M15" s="79">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" s="27" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="16" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B16" s="75" t="s">
@@ -9892,15 +10135,33 @@
       <c r="C16" s="66" t="s">
         <v>66</v>
       </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16" s="27"/>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
       <c r="I16" s="27"/>
+      <c r="J16" s="79">
+        <v>2</v>
+      </c>
       <c r="K16">
         <v>100</v>
       </c>
       <c r="L16" s="27"/>
+      <c r="M16" s="79">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>100</v>
+      </c>
       <c r="O16" s="27"/>
     </row>
     <row r="17" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -9910,15 +10171,33 @@
       <c r="C17" s="66" t="s">
         <v>56</v>
       </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17" s="27"/>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
       <c r="I17" s="27"/>
+      <c r="J17" s="79">
+        <v>0</v>
+      </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17" s="27"/>
+      <c r="M17" s="79">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>100</v>
+      </c>
       <c r="O17" s="27"/>
     </row>
     <row r="18" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -9928,16 +10207,34 @@
       <c r="C18" s="66" t="s">
         <v>147</v>
       </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18" s="27"/>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
       <c r="I18" s="27"/>
+      <c r="J18" s="79">
+        <v>1</v>
+      </c>
       <c r="K18">
         <v>50</v>
       </c>
       <c r="L18" s="27" t="s">
         <v>152</v>
+      </c>
+      <c r="M18" s="79">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>100</v>
       </c>
       <c r="O18" s="27"/>
     </row>
@@ -9946,16 +10243,36 @@
         <v>142</v>
       </c>
       <c r="C19" s="17"/>
+      <c r="D19">
+        <v>0</v>
+      </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19" s="17"/>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
       <c r="I19" s="17"/>
+      <c r="J19" s="79">
+        <v>0</v>
+      </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19" s="17"/>
-      <c r="O19" s="17"/>
+      <c r="M19" s="79">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>100</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="20" spans="2:15" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B20" s="62" t="s">
@@ -9972,15 +10289,33 @@
         <v>115</v>
       </c>
       <c r="C21" s="17"/>
+      <c r="D21">
+        <v>0</v>
+      </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21" s="17"/>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
       <c r="I21" s="17"/>
+      <c r="J21">
+        <v>0</v>
+      </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21" s="17"/>
+      <c r="M21">
+        <v>2</v>
+      </c>
+      <c r="N21">
+        <v>100</v>
+      </c>
       <c r="O21" s="17"/>
     </row>
     <row r="22" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -9988,15 +10323,33 @@
         <v>116</v>
       </c>
       <c r="C22" s="17"/>
+      <c r="D22">
+        <v>0</v>
+      </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22" s="17"/>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
       <c r="I22" s="17"/>
+      <c r="J22">
+        <v>0</v>
+      </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22" s="17"/>
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>100</v>
+      </c>
       <c r="O22" s="17"/>
     </row>
     <row r="23" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -10004,15 +10357,33 @@
         <v>117</v>
       </c>
       <c r="C23" s="17"/>
+      <c r="D23">
+        <v>0</v>
+      </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23" s="17"/>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
       <c r="I23" s="17"/>
+      <c r="J23">
+        <v>0</v>
+      </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23" s="17"/>
+      <c r="M23">
+        <v>2</v>
+      </c>
+      <c r="N23">
+        <v>100</v>
+      </c>
       <c r="O23" s="17"/>
     </row>
     <row r="24" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -10020,20 +10391,41 @@
         <v>118</v>
       </c>
       <c r="C24" s="17"/>
+      <c r="D24">
+        <v>0</v>
+      </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24" s="17"/>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
       <c r="I24" s="17"/>
+      <c r="J24">
+        <v>0</v>
+      </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24" s="17"/>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24">
+        <v>100</v>
+      </c>
       <c r="O24" s="17"/>
     </row>
     <row r="25" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B25" s="23"/>
       <c r="C25" s="17"/>
+      <c r="D25">
+        <v>0</v>
+      </c>
       <c r="E25">
         <v>0</v>
       </c>
@@ -10049,17 +10441,35 @@
       <c r="C26" s="66" t="s">
         <v>66</v>
       </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
       <c r="E26">
         <v>50</v>
       </c>
       <c r="F26" s="66" t="s">
         <v>122</v>
       </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>50</v>
+      </c>
       <c r="I26" s="27"/>
+      <c r="J26">
+        <v>4</v>
+      </c>
       <c r="K26">
         <v>100</v>
       </c>
       <c r="L26" s="27"/>
+      <c r="M26" s="79">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>100</v>
+      </c>
       <c r="O26" s="27"/>
     </row>
     <row r="27" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -10069,15 +10479,33 @@
       <c r="C27" s="66" t="s">
         <v>66</v>
       </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
       <c r="E27">
         <v>100</v>
       </c>
       <c r="F27" s="27"/>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>100</v>
+      </c>
       <c r="I27" s="27"/>
+      <c r="J27" s="79">
+        <v>0</v>
+      </c>
       <c r="K27">
         <v>100</v>
       </c>
       <c r="L27" s="27"/>
+      <c r="M27" s="79">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>100</v>
+      </c>
       <c r="O27" s="27"/>
     </row>
     <row r="28" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10087,26 +10515,38 @@
       <c r="C28" s="65" t="s">
         <v>66</v>
       </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
       <c r="E28">
         <v>100</v>
       </c>
       <c r="F28" s="17"/>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>100</v>
+      </c>
       <c r="I28" s="17"/>
+      <c r="J28" s="79">
+        <v>0</v>
+      </c>
       <c r="K28">
         <v>100</v>
       </c>
       <c r="L28" s="17"/>
+      <c r="M28" s="79">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>100</v>
+      </c>
       <c r="O28" s="17"/>
     </row>
     <row r="29" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="23"/>
       <c r="C29" s="17"/>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
       <c r="F29" s="17"/>
       <c r="I29" s="17"/>
       <c r="L29" s="17"/>
@@ -10126,12 +10566,27 @@
         <v>0</v>
       </c>
       <c r="F30" s="17"/>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
       <c r="I30" s="17"/>
+      <c r="J30" s="79">
+        <v>2</v>
+      </c>
       <c r="K30">
         <v>90</v>
       </c>
       <c r="L30" s="17" t="s">
         <v>153</v>
+      </c>
+      <c r="M30" s="79">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>100</v>
       </c>
       <c r="O30" s="17"/>
     </row>
@@ -10147,11 +10602,26 @@
         <v>0</v>
       </c>
       <c r="F31" s="17"/>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
       <c r="I31" s="17"/>
+      <c r="J31" s="79">
+        <v>2</v>
+      </c>
       <c r="K31">
         <v>100</v>
       </c>
       <c r="L31" s="17"/>
+      <c r="M31" s="79">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>100</v>
+      </c>
       <c r="O31" s="17"/>
     </row>
     <row r="32" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10168,14 +10638,31 @@
         <v>0</v>
       </c>
       <c r="F32" s="27"/>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
       <c r="I32" s="27"/>
+      <c r="J32" s="79">
+        <v>4</v>
+      </c>
       <c r="K32">
         <v>90</v>
       </c>
       <c r="L32" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="O32" s="27"/>
+        <v>159</v>
+      </c>
+      <c r="M32" s="79">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>100</v>
+      </c>
+      <c r="O32" s="27" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="33" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="72" t="s">
@@ -10189,14 +10676,31 @@
         <v>0</v>
       </c>
       <c r="F33" s="27"/>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
       <c r="I33" s="27"/>
+      <c r="J33" s="79">
+        <v>3</v>
+      </c>
       <c r="K33">
         <v>80</v>
       </c>
       <c r="L33" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="O33" s="27"/>
+      <c r="M33" s="79">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>80</v>
+      </c>
+      <c r="O33" s="27" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="34" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="72" t="s">
@@ -10210,12 +10714,29 @@
         <v>0</v>
       </c>
       <c r="F34" s="27"/>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
       <c r="I34" s="27"/>
+      <c r="J34" s="79">
+        <v>0</v>
+      </c>
       <c r="K34">
         <v>0</v>
       </c>
       <c r="L34" s="27"/>
-      <c r="O34" s="27"/>
+      <c r="M34" s="79">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>100</v>
+      </c>
+      <c r="O34" s="27" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="35" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="68" t="s">
@@ -10231,12 +10752,29 @@
         <v>0</v>
       </c>
       <c r="F35" s="27"/>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
       <c r="I35" s="27"/>
+      <c r="J35" s="79">
+        <v>2</v>
+      </c>
       <c r="K35">
         <v>80</v>
       </c>
       <c r="L35" s="27"/>
-      <c r="O35" s="27"/>
+      <c r="M35" s="79">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>100</v>
+      </c>
+      <c r="O35" s="27" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="36" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="69" t="s">
@@ -10252,14 +10790,31 @@
         <v>0</v>
       </c>
       <c r="F36" s="17"/>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
       <c r="I36" s="17"/>
+      <c r="J36" s="79">
+        <v>0</v>
+      </c>
       <c r="K36">
         <v>0</v>
       </c>
       <c r="L36" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="O36" s="17"/>
+      <c r="M36" s="79">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36" s="17" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="37" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="69" t="s">
@@ -10286,10 +10841,19 @@
       <c r="I37" s="17" t="s">
         <v>149</v>
       </c>
+      <c r="J37" s="79">
+        <v>1</v>
+      </c>
       <c r="K37">
         <v>100</v>
       </c>
       <c r="L37" s="17"/>
+      <c r="M37" s="79">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>100</v>
+      </c>
       <c r="O37" s="17"/>
     </row>
     <row r="38" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10297,40 +10861,133 @@
         <v>154</v>
       </c>
       <c r="C38" s="17"/>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
       <c r="F38" s="17"/>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
       <c r="I38" s="17"/>
+      <c r="J38" s="79">
+        <v>1</v>
+      </c>
       <c r="K38">
         <v>100</v>
       </c>
       <c r="L38" s="17"/>
+      <c r="M38" s="79">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>100</v>
+      </c>
       <c r="O38" s="17"/>
     </row>
     <row r="39" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C39" s="17"/>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
       <c r="F39" s="17"/>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
       <c r="I39" s="17"/>
+      <c r="J39" s="79">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
       <c r="L39" s="17"/>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>100</v>
+      </c>
       <c r="O39" s="17"/>
     </row>
     <row r="40" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C40" s="17"/>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
       <c r="F40" s="17"/>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
       <c r="I40" s="17"/>
+      <c r="J40" s="79">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
       <c r="L40" s="17"/>
+      <c r="M40">
+        <v>2</v>
+      </c>
+      <c r="N40">
+        <v>100</v>
+      </c>
       <c r="O40" s="17"/>
     </row>
     <row r="41" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="23"/>
       <c r="C41" s="17"/>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
       <c r="F41" s="17"/>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
       <c r="I41" s="17"/>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
       <c r="L41" s="17"/>
+      <c r="M41">
+        <v>2</v>
+      </c>
+      <c r="N41">
+        <v>100</v>
+      </c>
       <c r="O41" s="17"/>
     </row>
     <row r="42" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>